<commit_message>
update execl file and adding solving
</commit_message>
<xml_diff>
--- a/Trainingdata_sheet.xlsx
+++ b/Trainingdata_sheet.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="54">
   <si>
     <t>990 elements (max mesh size 0.09)</t>
   </si>
@@ -189,6 +189,12 @@
   </si>
   <si>
     <t>Ø2</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>3 layers [2, 1 , 1 ; 2, 1, 0.4; 2,1, 0.2]</t>
   </si>
 </sst>
 </file>
@@ -711,7 +717,7 @@
   <dimension ref="A1:P37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1308,44 +1314,92 @@
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>_16e__cell_anti_</v>
-      </c>
-      <c r="B20" s="1"/>
+        <v>2D_16e_adad_cell1_SNR20dB_50k</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C20" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="1"/>
+      <c r="D20" s="1">
+        <v>0.05</v>
+      </c>
       <c r="E20" s="1">
         <v>16</v>
       </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
+      <c r="F20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I20" s="1">
+        <v>1</v>
+      </c>
+      <c r="J20" t="s">
+        <v>37</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N20">
+        <v>20</v>
+      </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>_16e__cell_anti_</v>
-      </c>
-      <c r="B21" s="1"/>
+        <v>3D_16e_adad_cell1_SNR20dB_50k</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C21" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="1"/>
+      <c r="D21" s="1">
+        <v>0.05</v>
+      </c>
       <c r="E21" s="1">
         <v>16</v>
       </c>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
+      <c r="F21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I21" s="1">
+        <v>1</v>
+      </c>
+      <c r="J21" t="s">
+        <v>37</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N21">
+        <v>20</v>
+      </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="str">

</xml_diff>